<commit_message>
SHIP-3 I was able to craete mock data but I can not continue command 4  #### Step 4: Import prepared Data Processing Elements (DPE) data_proc_elem <- readxl::read_excel(here::here(paste0(folder_name, "/rmonize/data_proc_elem"), paste0("DPE_",dataset_name, ".xlsx")), sheet = 1)
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F0696-717F-429C-AE83-1E1283E8617E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94787687-A9BD-4CB4-A602-79BC2FDD9B3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="136">
   <si>
     <t>index</t>
   </si>
@@ -62,9 +62,6 @@
     <t>ncig1</t>
   </si>
   <si>
-    <t>quityear</t>
-  </si>
-  <si>
     <t>menostat_s0</t>
   </si>
   <si>
@@ -95,15 +92,9 @@
     <t>atc_m01a_s0</t>
   </si>
   <si>
-    <t>herz_01 (START-4)</t>
-  </si>
-  <si>
     <t>inc_diab_s0</t>
   </si>
   <si>
-    <t>krebs_01 (START-4)</t>
-  </si>
-  <si>
     <t>mort_all</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
   </si>
   <si>
     <t>average number of cigarettes smoked per day</t>
-  </si>
-  <si>
-    <t>year in which smoking was quit</t>
   </si>
   <si>
     <t>male</t>
@@ -335,15 +323,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t xml:space="preserve">inc_mi_s0 (START-0) </t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>inc_stroke_s0 (START-0)</t>
-  </si>
-  <si>
     <t>Incident stroke</t>
   </si>
   <si>
@@ -407,9 +386,6 @@
     <t>Have you ever had a heart surgery?</t>
   </si>
   <si>
-    <t>inc_stroke_s0(START-0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID </t>
   </si>
   <si>
@@ -431,22 +407,31 @@
     <t>ang_01b(START-4)</t>
   </si>
   <si>
-    <t xml:space="preserve">inc_mi_s0(START-0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mi_03b5(START-4)  </t>
-  </si>
-  <si>
-    <t>herz_01(START-4)</t>
-  </si>
-  <si>
-    <t>krebs_01(START-4)</t>
-  </si>
-  <si>
     <t>packyears[number of cigarettes per day * years smoked/20]</t>
   </si>
   <si>
     <t>uncertain status (not yet 12 months without menstruation and natural menopause)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inc_mi_s0 </t>
+  </si>
+  <si>
+    <t>inc_stroke_s0</t>
+  </si>
+  <si>
+    <t>herz_01</t>
+  </si>
+  <si>
+    <t>krebs_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inc_stroke_s0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">herz_01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">krebs_01 </t>
   </si>
 </sst>
 </file>
@@ -940,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,10 +957,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -983,10 +968,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,10 +979,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1005,10 +990,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1027,10 +1012,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1038,10 +1023,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1049,35 +1034,35 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1085,194 +1070,194 @@
         <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>124</v>
+        <v>114</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -1280,142 +1265,142 @@
         <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>133</v>
+      <c r="B34" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>132</v>
+      <c r="B35" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" t="s">
-        <v>104</v>
+        <v>23</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>107</v>
+        <v>24</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>108</v>
+      <c r="C41" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>138</v>
+        <v>26</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -1423,88 +1408,44 @@
         <v>27</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" t="s">
-        <v>33</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D45" t="s">
-        <v>102</v>
-      </c>
+      <c r="C45" s="12"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" t="s">
-        <v>33</v>
-      </c>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D48" s="9"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="12"/>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="9"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="9"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="9"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="9"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="9"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="9"/>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="9"/>
-    </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="3"/>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1516,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1579,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1590,7 +1531,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1601,7 +1542,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1612,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1623,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1634,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1656,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1667,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1678,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1689,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1700,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1711,7 +1652,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1722,7 +1663,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1733,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1744,7 +1685,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1755,1054 +1696,1054 @@
         <v>9</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="10">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="10">
         <v>1</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="10">
         <v>99</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="10">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="10">
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="10">
         <v>97</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="28">
         <v>98</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="28">
         <v>99</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="10">
         <v>1</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="10">
         <v>0</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="10">
         <v>1</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B35" s="23">
         <v>1</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B36" s="23">
         <v>2</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B37" s="23">
         <v>8</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B38" s="23">
         <v>9</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B39" s="23">
         <v>1</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B40" s="23">
         <v>2</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B41" s="23">
         <v>8</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B42" s="23">
         <v>9</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B43" s="23">
         <v>1</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B44" s="23">
         <v>2</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B45" s="23">
         <v>8</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B46" s="23">
         <v>9</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="10">
         <v>1</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="10">
         <v>2</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="10">
         <v>8</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="10">
         <v>9</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B51" s="10">
         <v>1</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B52" s="10">
         <v>2</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B53" s="10">
         <v>8</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B54" s="10">
         <v>9</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B55" s="10">
         <v>1</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B56" s="10">
         <v>2</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B57" s="10">
         <v>8</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B58" s="10">
         <v>9</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B61" s="10">
         <v>8</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B62" s="10">
         <v>9</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B63" s="10">
         <v>1</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B64" s="10">
         <v>2</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B65" s="10">
         <v>8</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B66" s="10">
         <v>9</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B67" s="10">
         <v>1</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B68" s="10">
         <v>2</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B69" s="10">
         <v>8</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B70" s="10">
         <v>9</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B73" s="10">
         <v>8</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B74" s="10">
         <v>9</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B75" s="10">
         <v>1</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B76" s="10">
         <v>2</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B77" s="10">
         <v>8</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B78" s="10">
         <v>9</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B79" s="10">
         <v>1</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B80" s="10">
         <v>2</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B81" s="10">
         <v>8</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B82" s="10">
         <v>9</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B83" s="10">
         <v>0</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B84" s="10">
         <v>1</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B89" s="25">
         <v>1</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B90" s="25">
         <v>0</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B91" s="25">
         <v>998</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B92" s="25">
         <v>999</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B93" s="25">
         <v>1</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B94" s="25">
         <v>0</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B95" s="25">
         <v>998</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B96" s="25">
         <v>999</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B97" s="10">
         <v>0</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B98" s="10">
         <v>1</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B99" s="10">
         <v>0</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B100" s="10">
         <v>1</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B102" s="10">
         <v>0</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B103" s="10">
         <v>998</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B104" s="10">
         <v>999</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B105" s="24">
         <v>0</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B106" s="24">
         <v>1</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B108" s="10">
         <v>0</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B109" s="10">
         <v>998</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B110" s="10">
         <v>999</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B111" s="10">
         <v>0</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B112" s="10">
         <v>1</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B113" s="24">
         <v>0</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B114" s="24">
         <v>1</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B115" s="10">
         <v>0</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SHIP-3 EDU-I have placed all potential variable in the comparison table but unfortunately heatmap could don update the variables. TOT_PA_QX;this is in categories and I dont know if it best we calculate METhr/day from categories. will discuss that with Kathi. Employment;done as suggested IMMIGRATION:done as suggested TOBACCO_D;done as suggested MENOPAUSE;Recoded the variable MI and Angina;Names corrected
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECF5F3-44C4-441B-A034-4ECE10562220}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88239E-63E4-481C-81BB-9478CBA6B1AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="151">
   <si>
     <t>index</t>
   </si>
@@ -398,12 +398,6 @@
     <t>medication:statins</t>
   </si>
   <si>
-    <t>mi_03b5(START-4)</t>
-  </si>
-  <si>
-    <t>ang_01b(START-4)</t>
-  </si>
-  <si>
     <t>packyears[number of cigarettes per day * years smoked/20]</t>
   </si>
   <si>
@@ -432,6 +426,57 @@
   </si>
   <si>
     <t>ang_01</t>
+  </si>
+  <si>
+    <t>mi_03b5_4</t>
+  </si>
+  <si>
+    <t>ang_01b_4</t>
+  </si>
+  <si>
+    <t>nojob</t>
+  </si>
+  <si>
+    <t>group of job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retired </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Student </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> professional student </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> unemployed </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> unemployed, in retraining </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zero short-time work </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> housewife/househusband </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wher-/Civilian service </t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>npipes</t>
+  </si>
+  <si>
+    <t>How many cigars or cigarillos/ day do you smoke on average?</t>
+  </si>
+  <si>
+    <t>ncigard</t>
+  </si>
+  <si>
+    <t>How many pipes/ day do you smoke on average?</t>
   </si>
 </sst>
 </file>
@@ -936,17 +981,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1029,166 +1074,166 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+    <row r="16" spans="1:4" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C16" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="D16" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C19" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="D19" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C20" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="D20" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="D21" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D22" t="s">
         <v>98</v>
@@ -1196,10 +1241,10 @@
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>98</v>
@@ -1207,10 +1252,10 @@
     </row>
     <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>98</v>
@@ -1218,10 +1263,10 @@
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
         <v>98</v>
@@ -1229,10 +1274,10 @@
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>98</v>
@@ -1240,10 +1285,10 @@
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
         <v>98</v>
@@ -1251,120 +1296,120 @@
     </row>
     <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="D34" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C37" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="2" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="D38" t="s">
         <v>98</v>
@@ -1372,43 +1417,43 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>102</v>
+        <v>127</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>103</v>
+        <v>128</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="D40" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>106</v>
+        <v>23</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
         <v>98</v>
@@ -1416,47 +1461,80 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="12"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="9"/>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="9"/>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="9"/>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="9"/>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="9"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="9"/>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="3"/>
+      <c r="C48" s="12"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="9"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="9"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="9"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="9"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="9"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="9"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,690 +1789,690 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
+      <c r="A22" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B22" s="10">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
+      <c r="A23" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B24" s="10">
-        <v>2</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B25" s="10">
-        <v>99</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>127</v>
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>14</v>
+      <c r="A26" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B26" s="10">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>14</v>
+      <c r="A27" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B27" s="10">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="B28" s="10">
-        <v>97</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="28">
-        <v>98</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="28">
-        <v>99</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="10">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="10">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="10">
+        <v>2</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="10">
+        <v>99</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="10">
+        <v>1</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="10">
+        <v>97</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="28">
+        <v>98</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="28">
+        <v>99</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="10">
-        <v>1</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="10">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B42" s="10">
         <v>0</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="10">
-        <v>1</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B43" s="10">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="23">
-        <v>1</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="23">
-        <v>2</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="23">
-        <v>8</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="23">
-        <v>9</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="23">
-        <v>1</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="23">
-        <v>2</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="23">
-        <v>8</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="23">
-        <v>9</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" s="23">
-        <v>1</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="23">
+        <v>8</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="23">
+        <v>9</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="23">
+        <v>1</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="23">
+        <v>2</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="23">
+        <v>8</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="23">
+        <v>9</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B52" s="23">
+        <v>1</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="23">
+        <v>2</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="23">
+        <v>8</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="23">
         <v>9</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C55" s="21" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="10">
-        <v>1</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="10">
-        <v>2</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="10">
-        <v>8</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="10">
-        <v>9</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="10">
-        <v>1</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="10">
-        <v>2</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="10">
-        <v>8</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="10">
-        <v>9</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="10">
-        <v>1</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B56" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B57" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B58" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="B59" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B60" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B61" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B62" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B63" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B64" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B66" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B67" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B68" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B69" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B70" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B71" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B72" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B73" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B74" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B76" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B77" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B78" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B79" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B80" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B81" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B82" s="10">
+        <v>8</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="10">
         <v>9</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C83" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B83" s="10">
-        <v>0</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>20</v>
+      <c r="A84" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B84" s="10">
         <v>1</v>
@@ -2403,357 +2481,456 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B85" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B85" s="10">
+        <v>2</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B86" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B86" s="10">
+        <v>8</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B87" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B87" s="10">
+        <v>9</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="B88" s="10">
+        <v>1</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B89" s="25">
-        <v>1</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="B89" s="10">
+        <v>2</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B90" s="25">
-        <v>0</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>91</v>
+        <v>75</v>
+      </c>
+      <c r="B90" s="10">
+        <v>8</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B91" s="10">
+        <v>9</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" s="10">
+        <v>0</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" s="10">
+        <v>1</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="25">
-        <v>998</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="25">
-        <v>999</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B93" s="25">
-        <v>1</v>
-      </c>
-      <c r="C93" s="15" t="s">
+      <c r="B98" s="25">
+        <v>1</v>
+      </c>
+      <c r="C98" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B94" s="25">
-        <v>0</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B95" s="25">
-        <v>998</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B96" s="25">
-        <v>999</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B97" s="10">
-        <v>0</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D97" s="5"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B98" s="10">
-        <v>1</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B99" s="10">
+        <v>89</v>
+      </c>
+      <c r="B99" s="25">
         <v>0</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="15" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B100" s="10">
-        <v>1</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>54</v>
+        <v>89</v>
+      </c>
+      <c r="B100" s="25">
+        <v>998</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B101" s="10">
-        <v>1</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="B101" s="25">
+        <v>999</v>
+      </c>
+      <c r="C101" s="15" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B102" s="10">
-        <v>0</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>58</v>
+      <c r="B102" s="25">
+        <v>1</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B103" s="10">
-        <v>998</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>92</v>
+      <c r="B103" s="25">
+        <v>0</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B104" s="10">
-        <v>999</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>95</v>
+      <c r="B104" s="25">
+        <v>998</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B105" s="24">
+        <v>133</v>
+      </c>
+      <c r="B105" s="25">
+        <v>999</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="10">
         <v>0</v>
       </c>
-      <c r="C105" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="24">
-        <v>1</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="C106" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>134</v>
+      <c r="A107" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>87</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D107" s="5"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B108" s="10">
         <v>0</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B109" s="10">
-        <v>998</v>
+        <v>1</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B110" s="10">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B111" s="10">
         <v>0</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B112" s="10">
-        <v>1</v>
+        <v>998</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B113" s="24">
-        <v>0</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>91</v>
+        <v>131</v>
+      </c>
+      <c r="B113" s="10">
+        <v>999</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B114" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B115" s="10">
-        <v>0</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>58</v>
+        <v>23</v>
+      </c>
+      <c r="B115" s="24">
+        <v>1</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B116" s="10">
+        <v>1</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B117" s="10">
+        <v>0</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B118" s="10">
+        <v>998</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" s="10">
+        <v>999</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120" s="10">
+        <v>0</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" s="10">
+        <v>1</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" s="24">
+        <v>0</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" s="24">
+        <v>1</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B116" s="10">
-        <v>1</v>
-      </c>
-      <c r="C116" s="13" t="s">
+      <c r="B124" s="10">
+        <v>0</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B125" s="10">
+        <v>1</v>
+      </c>
+      <c r="C125" s="13" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SHIP-3 Education-Changed to undetermine Physical activity-Changed to undetermine
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_SHIP_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88239E-63E4-481C-81BB-9478CBA6B1AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CD82FB-A512-42D9-B77F-ABA2EF082B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="159">
   <si>
     <t>index</t>
   </si>
@@ -477,6 +477,30 @@
   </si>
   <si>
     <t>How many pipes/ day do you smoke on average?</t>
+  </si>
+  <si>
+    <t>sportwi1</t>
+  </si>
+  <si>
+    <t>sportwi3</t>
+  </si>
+  <si>
+    <t>sportso1</t>
+  </si>
+  <si>
+    <t>sportso3</t>
+  </si>
+  <si>
+    <t>Which of the following items best describes your sports activity in winter time?</t>
+  </si>
+  <si>
+    <t>How often do you do sport in summer time?</t>
+  </si>
+  <si>
+    <t>Which of the following items best describes your sports activity in summer time?</t>
+  </si>
+  <si>
+    <t>How often do you do sport in winter time?</t>
   </si>
 </sst>
 </file>
@@ -981,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,232 +1076,232 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="D11" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="D12" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+    <row r="20" spans="2:4" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C20" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="D20" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>98</v>
@@ -1285,10 +1309,10 @@
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>98</v>
@@ -1296,10 +1320,10 @@
     </row>
     <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
         <v>98</v>
@@ -1307,10 +1331,10 @@
     </row>
     <row r="29" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>98</v>
@@ -1318,10 +1342,10 @@
     </row>
     <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
         <v>98</v>
@@ -1329,131 +1353,131 @@
     </row>
     <row r="31" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+      <c r="D37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="D38" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+    <row r="41" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="D42" t="s">
         <v>98</v>
@@ -1461,32 +1485,32 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>103</v>
+        <v>127</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D43" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D45" t="s">
         <v>98</v>
@@ -1494,47 +1518,91 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="12"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D51" s="9"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="12"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D53" s="9"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="9"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="9"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D59" s="9"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D61" s="9"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="3"/>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="9"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="9"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1546,7 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:A30"/>
     </sheetView>
   </sheetViews>

</xml_diff>